<commit_message>
Anh add Edit User Profile TC  16/07/2019
</commit_message>
<xml_diff>
--- a/src/test/Data/ResultDemo.xlsx
+++ b/src/test/Data/ResultDemo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="26">
   <si>
     <t>TC_ID</t>
   </si>
@@ -87,6 +87,12 @@
   <si>
     <t>Verify that user cannot login with an email of user was blocked</t>
   </si>
+  <si>
+    <t>TC_REQ_UPM_Update_03_01</t>
+  </si>
+  <si>
+    <t>Verify that 'Edit success!' message displays when user updates information successfully</t>
+  </si>
 </sst>
 </file>
 
@@ -109,7 +115,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="265">
+  <fills count="269">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1431,8 +1437,28 @@
         <fgColor indexed="10"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="266">
+  <borders count="270">
     <border>
       <left/>
       <right/>
@@ -2643,12 +2669,30 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="2" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="135">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="1"/>
     <xf applyBorder="true" applyFill="true" borderId="5" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
@@ -2780,8 +2824,10 @@
     <xf applyBorder="true" applyFill="true" borderId="257" fillId="256" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="261" fillId="258" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="261" fillId="260" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="262" borderId="265" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="264" borderId="265" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="265" fillId="262" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="265" fillId="264" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="266" borderId="269" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="268" borderId="269" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="20" name="Input" xfId="1"/>
@@ -3097,7 +3143,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -3106,7 +3152,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="31.0234375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="71.12890625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="78.8984375" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="9.921875" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="5.44921875" collapsed="true"/>
   </cols>
@@ -3841,14 +3887,25 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="s" s="131">
+      <c r="A67" s="131" t="s">
         <v>4</v>
       </c>
-      <c r="B67" t="s" s="131">
+      <c r="B67" s="131" t="s">
         <v>5</v>
       </c>
-      <c r="C67" t="s" s="132">
+      <c r="C67" s="132" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="133">
+        <v>24</v>
+      </c>
+      <c r="B68" t="s" s="133">
+        <v>25</v>
+      </c>
+      <c r="C68" t="s" s="134">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Anh add Edit User Profile TC  17/07/2019
</commit_message>
<xml_diff>
--- a/src/test/Data/ResultDemo.xlsx
+++ b/src/test/Data/ResultDemo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="42">
   <si>
     <t>TC_ID</t>
   </si>
@@ -93,6 +93,54 @@
   <si>
     <t>Verify that 'Edit success!' message displays when user updates information successfully</t>
   </si>
+  <si>
+    <t>TC_REQ_UPM_Update_04_01</t>
+  </si>
+  <si>
+    <t>Verify that 'Please enter your name' red message displays when leaving Name field blank</t>
+  </si>
+  <si>
+    <t>TC_REQ_UPM_Update_04_02</t>
+  </si>
+  <si>
+    <t>Verify that 'Please enter your company' red message displays when leaving Company field blank</t>
+  </si>
+  <si>
+    <t>TC_REQ_UPM_Update_04_03</t>
+  </si>
+  <si>
+    <t>Verify that 'Please enter your phone' red message displays when leaving Phone field blank</t>
+  </si>
+  <si>
+    <t>TC_REQ_UPM_Update_04_04</t>
+  </si>
+  <si>
+    <t>Verify that 'Only numbers 0-9' red message displays when user enters any letters into Phone field</t>
+  </si>
+  <si>
+    <t>TC_REQ_UPM_Update_04_05</t>
+  </si>
+  <si>
+    <t>Verify that 'Phone is 10-14 numbers' red message displays above Phone filed when user enters 3 numbers into Phone field</t>
+  </si>
+  <si>
+    <t>TC_REQ_UPM_Update_04_06</t>
+  </si>
+  <si>
+    <t>Verify that 'Phone is 10-14 numbers' red message displays above Phone filed when user enters 9 numbers into Phone field</t>
+  </si>
+  <si>
+    <t>TC_REQ_UPM_Update_04_07</t>
+  </si>
+  <si>
+    <t>Verify that 'Phone is 10-14 numbers' red message displays above Phone filed when user enters 15 numbers into Phone field</t>
+  </si>
+  <si>
+    <t>TC_REQ_UPM_Update_04_08</t>
+  </si>
+  <si>
+    <t>Verify that 'Phone is 10-14 numbers' red message displays above Phone filed when user enters 19 numbers into Phone field</t>
+  </si>
 </sst>
 </file>
 
@@ -115,7 +163,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="269">
+  <fills count="441">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1457,8 +1505,868 @@
         <fgColor indexed="42"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="270">
+  <borders count="442">
     <border>
       <left/>
       <right/>
@@ -2687,12 +3595,786 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="2" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="221">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="1"/>
     <xf applyBorder="true" applyFill="true" borderId="5" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
@@ -2826,8 +4508,94 @@
     <xf applyBorder="true" applyFill="true" borderId="261" fillId="260" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="265" fillId="262" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="265" fillId="264" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="266" borderId="269" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="268" borderId="269" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="269" fillId="266" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="269" fillId="268" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="273" fillId="270" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="273" fillId="272" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="277" fillId="274" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="277" fillId="276" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="281" fillId="278" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="281" fillId="280" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="285" fillId="282" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="285" fillId="284" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="289" fillId="286" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="289" fillId="288" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="293" fillId="290" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="293" fillId="292" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="297" fillId="294" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="297" fillId="296" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="301" fillId="298" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="301" fillId="300" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="305" fillId="302" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="305" fillId="304" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="309" fillId="306" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="309" fillId="308" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="313" fillId="310" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="313" fillId="312" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="317" fillId="314" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="317" fillId="316" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="321" fillId="318" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="321" fillId="320" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="325" fillId="322" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="325" fillId="324" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="329" fillId="326" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="329" fillId="328" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="333" fillId="330" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="333" fillId="332" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="337" fillId="334" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="337" fillId="336" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="341" fillId="338" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="341" fillId="340" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="345" fillId="342" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="345" fillId="344" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="349" fillId="346" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="349" fillId="348" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="353" fillId="350" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="353" fillId="352" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="357" fillId="354" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="357" fillId="356" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="361" fillId="358" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="361" fillId="360" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="365" fillId="362" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="365" fillId="364" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="369" fillId="366" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="369" fillId="368" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="373" fillId="370" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="373" fillId="372" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="377" fillId="374" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="377" fillId="376" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="381" fillId="378" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="381" fillId="380" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="385" fillId="382" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="385" fillId="384" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="389" fillId="386" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="389" fillId="388" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="393" fillId="390" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="393" fillId="392" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="397" fillId="394" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="397" fillId="396" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="401" fillId="398" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="401" fillId="400" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="405" fillId="402" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="405" fillId="404" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="409" fillId="406" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="409" fillId="408" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="413" fillId="410" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="413" fillId="412" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="417" fillId="414" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="417" fillId="416" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="421" fillId="418" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="421" fillId="420" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="425" fillId="422" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="425" fillId="424" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="429" fillId="426" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="429" fillId="428" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="433" fillId="430" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="433" fillId="432" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="437" fillId="434" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="437" fillId="436" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="438" borderId="441" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="440" borderId="441" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="20" name="Input" xfId="1"/>
@@ -3143,7 +4911,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -3152,7 +4920,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="31.0234375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="78.8984375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="111.46484375" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="9.921875" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="5.44921875" collapsed="true"/>
   </cols>
@@ -3898,14 +5666,487 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="s" s="133">
+      <c r="A68" s="133" t="s">
         <v>24</v>
       </c>
-      <c r="B68" t="s" s="133">
+      <c r="B68" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="C68" t="s" s="134">
-        <v>9</v>
+      <c r="C68" s="134" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="135" t="s">
+        <v>7</v>
+      </c>
+      <c r="B69" s="135" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" s="136" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="137" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70" s="137" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" s="138" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="139" t="s">
+        <v>12</v>
+      </c>
+      <c r="B71" s="139" t="s">
+        <v>13</v>
+      </c>
+      <c r="C71" s="140" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="141" t="s">
+        <v>14</v>
+      </c>
+      <c r="B72" s="141" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" s="142" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="143" t="s">
+        <v>16</v>
+      </c>
+      <c r="B73" s="143" t="s">
+        <v>17</v>
+      </c>
+      <c r="C73" s="144" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="145" t="s">
+        <v>18</v>
+      </c>
+      <c r="B74" s="145" t="s">
+        <v>19</v>
+      </c>
+      <c r="C74" s="146" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="147" t="s">
+        <v>20</v>
+      </c>
+      <c r="B75" s="147" t="s">
+        <v>21</v>
+      </c>
+      <c r="C75" s="148" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="149" t="s">
+        <v>22</v>
+      </c>
+      <c r="B76" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="C76" s="150" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="151" t="s">
+        <v>4</v>
+      </c>
+      <c r="B77" s="151" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" s="152" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="153" t="s">
+        <v>24</v>
+      </c>
+      <c r="B78" s="153" t="s">
+        <v>25</v>
+      </c>
+      <c r="C78" s="154" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="155" t="s">
+        <v>26</v>
+      </c>
+      <c r="B79" s="155" t="s">
+        <v>27</v>
+      </c>
+      <c r="C79" s="156" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="157" t="s">
+        <v>28</v>
+      </c>
+      <c r="B80" s="157" t="s">
+        <v>29</v>
+      </c>
+      <c r="C80" s="158" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="159" t="s">
+        <v>24</v>
+      </c>
+      <c r="B81" s="159" t="s">
+        <v>25</v>
+      </c>
+      <c r="C81" s="160" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="161" t="s">
+        <v>26</v>
+      </c>
+      <c r="B82" s="161" t="s">
+        <v>27</v>
+      </c>
+      <c r="C82" s="162" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="163" t="s">
+        <v>28</v>
+      </c>
+      <c r="B83" s="163" t="s">
+        <v>29</v>
+      </c>
+      <c r="C83" s="164" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="165" t="s">
+        <v>24</v>
+      </c>
+      <c r="B84" s="165" t="s">
+        <v>25</v>
+      </c>
+      <c r="C84" s="166" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="167" t="s">
+        <v>26</v>
+      </c>
+      <c r="B85" s="167" t="s">
+        <v>27</v>
+      </c>
+      <c r="C85" s="168" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="169" t="s">
+        <v>28</v>
+      </c>
+      <c r="B86" s="169" t="s">
+        <v>29</v>
+      </c>
+      <c r="C86" s="170" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="171" t="s">
+        <v>30</v>
+      </c>
+      <c r="B87" s="171" t="s">
+        <v>31</v>
+      </c>
+      <c r="C87" s="172" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="173" t="s">
+        <v>24</v>
+      </c>
+      <c r="B88" s="173" t="s">
+        <v>25</v>
+      </c>
+      <c r="C88" s="174" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="175" t="s">
+        <v>7</v>
+      </c>
+      <c r="B89" s="175" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" s="176" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="177" t="s">
+        <v>10</v>
+      </c>
+      <c r="B90" s="177" t="s">
+        <v>11</v>
+      </c>
+      <c r="C90" s="178" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="179" t="s">
+        <v>24</v>
+      </c>
+      <c r="B91" s="179" t="s">
+        <v>25</v>
+      </c>
+      <c r="C91" s="180" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="181" t="s">
+        <v>26</v>
+      </c>
+      <c r="B92" s="181" t="s">
+        <v>27</v>
+      </c>
+      <c r="C92" s="182" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="183" t="s">
+        <v>28</v>
+      </c>
+      <c r="B93" s="183" t="s">
+        <v>29</v>
+      </c>
+      <c r="C93" s="184" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="185" t="s">
+        <v>30</v>
+      </c>
+      <c r="B94" s="185" t="s">
+        <v>31</v>
+      </c>
+      <c r="C94" s="186" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="187" t="s">
+        <v>24</v>
+      </c>
+      <c r="B95" s="187" t="s">
+        <v>25</v>
+      </c>
+      <c r="C95" s="188" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="189" t="s">
+        <v>26</v>
+      </c>
+      <c r="B96" s="189" t="s">
+        <v>27</v>
+      </c>
+      <c r="C96" s="190" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="191" t="s">
+        <v>28</v>
+      </c>
+      <c r="B97" s="191" t="s">
+        <v>29</v>
+      </c>
+      <c r="C97" s="192" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="193" t="s">
+        <v>30</v>
+      </c>
+      <c r="B98" s="193" t="s">
+        <v>31</v>
+      </c>
+      <c r="C98" s="194" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="195" t="s">
+        <v>32</v>
+      </c>
+      <c r="B99" s="195" t="s">
+        <v>33</v>
+      </c>
+      <c r="C99" s="196" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="197" t="s">
+        <v>4</v>
+      </c>
+      <c r="B100" s="197" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" s="198" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="199" t="s">
+        <v>22</v>
+      </c>
+      <c r="B101" s="199" t="s">
+        <v>23</v>
+      </c>
+      <c r="C101" s="200" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="201" t="s">
+        <v>34</v>
+      </c>
+      <c r="B102" s="201" t="s">
+        <v>35</v>
+      </c>
+      <c r="C102" s="202" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="203" t="s">
+        <v>24</v>
+      </c>
+      <c r="B103" s="203" t="s">
+        <v>25</v>
+      </c>
+      <c r="C103" s="204" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="205" t="s">
+        <v>26</v>
+      </c>
+      <c r="B104" s="205" t="s">
+        <v>27</v>
+      </c>
+      <c r="C104" s="206" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="207" t="s">
+        <v>28</v>
+      </c>
+      <c r="B105" s="207" t="s">
+        <v>29</v>
+      </c>
+      <c r="C105" s="208" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="209" t="s">
+        <v>30</v>
+      </c>
+      <c r="B106" s="209" t="s">
+        <v>31</v>
+      </c>
+      <c r="C106" s="210" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="211" t="s">
+        <v>32</v>
+      </c>
+      <c r="B107" s="211" t="s">
+        <v>33</v>
+      </c>
+      <c r="C107" s="212" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="213" t="s">
+        <v>34</v>
+      </c>
+      <c r="B108" s="213" t="s">
+        <v>35</v>
+      </c>
+      <c r="C108" s="214" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="215" t="s">
+        <v>36</v>
+      </c>
+      <c r="B109" s="215" t="s">
+        <v>37</v>
+      </c>
+      <c r="C109" s="216" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="217" t="s">
+        <v>38</v>
+      </c>
+      <c r="B110" s="217" t="s">
+        <v>39</v>
+      </c>
+      <c r="C110" s="218" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s" s="219">
+        <v>40</v>
+      </c>
+      <c r="B111" t="s" s="219">
+        <v>41</v>
+      </c>
+      <c r="C111" t="s" s="220">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>